<commit_message>
AFDP-2369 Modified the drools file for next possible queue.
Former-commit-id: 7e8776e04517550935c26478460a435328cfc50e
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-next-possible-queues-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-next-possible-queues-rules.xlsx
@@ -26,7 +26,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0" shapeId="0">
+    <comment ref="B17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0">
+    <comment ref="D17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>RuleSet</t>
   </si>
@@ -120,19 +120,51 @@
     <t>$model.setNextPossibleQueues($param);</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>$model.businessObject.queue.name.equals("$param")</t>
-  </si>
-  <si>
     <t>com.armedia.acm.plugins.businessprocess.model.NextPossibleQueuesModel</t>
   </si>
   <si>
     <t>$model: NextPossibleQueuesModel</t>
+  </si>
+  <si>
+    <t>com.armedia.acm.plugins.casefile.model.CaseFile</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.EvaluationContext</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.Expression</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.ExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.standard.SpelExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.support.StandardEvaluationContext</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>eval(evalSpring("$param", $model))</t>
+  </si>
+  <si>
+    <t>queue?.name.equals("*")</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>function Boolean evalSpring(String expression, NextPossibleQueuesModel model)
+{
+    ExpressionParser ep = new SpelExpressionParser();
+    Expression exp = ep.parseExpression(expression);
+    EvaluationContext ec = new StandardEvaluationContext();
+ CaseFile caseFile = (CaseFile) model.getBusinessObject();
+    Boolean evaluated = exp.getValue(ec, caseFile, Boolean.class);
+    return evaluated;
+}</t>
   </si>
 </sst>
 </file>
@@ -142,7 +174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -164,6 +196,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -387,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -400,7 +438,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -424,6 +461,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -986,10 +1029,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1033,7 +1076,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1042,11 +1085,11 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>4</v>
+      <c r="C4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1055,8 +1098,12 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>17</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1064,76 +1111,128 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3"/>
+      <c r="C6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>7</v>
+      <c r="C7" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="9"/>
+      <c r="C8" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="C9" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="171" x14ac:dyDescent="0.45">
+      <c r="C10" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+    </row>
+    <row r="12" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C16" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="114" x14ac:dyDescent="0.45">
-      <c r="A10" s="12" t="s">
+    <row r="17" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+      <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17" t="s">
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="C18" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
AFDP-2521 Added default return queue to the 'NextPossibleQueuesModel'.
Former-commit-id: cd3e3f4a9d04f693dfb453f259ec10b1ce31347c
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-next-possible-queues-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-next-possible-queues-rules.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>RuleSet</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>queue.name.equals("no-such-queue")</t>
+  </si>
+  <si>
+    <t>$model.setDefaultNextQueue("$param");</t>
+  </si>
+  <si>
+    <t>Default next queue</t>
+  </si>
+  <si>
+    <t>$model.setDefaultReturnQueue($param);</t>
   </si>
 </sst>
 </file>
@@ -204,7 +213,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +262,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAC090"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -425,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -467,6 +482,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1031,8 +1049,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1042,7 +1060,7 @@
     <col min="3" max="3" width="69.53125"/>
     <col min="4" max="4" width="70.6640625"/>
     <col min="5" max="5" width="35.73046875"/>
-    <col min="6" max="6" width="24.1328125"/>
+    <col min="6" max="6" width="36.3984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.59765625"/>
     <col min="8" max="1025" width="8.73046875"/>
   </cols>
@@ -1163,8 +1181,12 @@
       <c r="D11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="E11" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>4</v>
+      </c>
       <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -1172,8 +1194,6 @@
       <c r="B12" s="16"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
       <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -1181,6 +1201,8 @@
         <v>5</v>
       </c>
       <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C14" s="5" t="s">
@@ -1189,12 +1211,20 @@
       <c r="D14" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="E14" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="9"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C16" s="23" t="s">
@@ -1203,8 +1233,14 @@
       <c r="D16" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+      <c r="E16" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="114" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -1217,8 +1253,14 @@
       <c r="D17" s="14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="15"/>
       <c r="B18" s="16" t="s">
         <v>10</v>
@@ -1229,8 +1271,14 @@
       <c r="D18" s="18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E18" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C19" s="17"/>
       <c r="D19" s="18"/>
     </row>

</xml_diff>